<commit_message>
First test run failed, but the code is now ready for commit.
</commit_message>
<xml_diff>
--- a/Intern_project/Fundsquare_webscrapping Project/Fundsquare first test.xlsx
+++ b/Intern_project/Fundsquare_webscrapping Project/Fundsquare first test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ukesh\Coding Shinobi\Coding-Shinobi\Intern_project\Fundsquare_webscrapping Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3F8CA8-95BA-4C6D-95B3-1F4748D41415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DB95F0-DFB3-4344-B2D7-8EFAD6358D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Final prototype commit message
</commit_message>
<xml_diff>
--- a/Intern_project/Fundsquare_webscrapping Project/Fundsquare first test.xlsx
+++ b/Intern_project/Fundsquare_webscrapping Project/Fundsquare first test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ukesh\Coding Shinobi\Coding-Shinobi\Intern_project\Fundsquare_webscrapping Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C7309C-77F1-4C2D-BC6B-0958A31F285E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F22636F-D325-461F-A12F-B3797D709BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Fundsquare_URL</t>
   </si>
@@ -45,12 +45,90 @@
   <si>
     <t>https://www.fundsquare.net/security/information?idInstr=2509951</t>
   </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=1838003</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=328033</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=259953</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=331292</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=383771</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=68003</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=2505611</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=433005</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=369070</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=383770</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/summary?idInstr=213178</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=209254</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=209272</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=280385</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=140388</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=236383</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=370126</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/summary?idInstr=399090</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/summary?idInstr=322611</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=430448</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=2402915</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=2402919</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=2402907</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=388103</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=437621</t>
+  </si>
+  <si>
+    <t>https://www.fundsquare.net/security/information?idInstr=341001</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -74,6 +152,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -117,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -127,6 +211,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -350,7 +440,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -408,60 +498,224 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
-    <row r="29" x14ac:dyDescent="0.2"/>
-    <row r="30" x14ac:dyDescent="0.2"/>
-    <row r="31" x14ac:dyDescent="0.2"/>
-    <row r="32" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
-    <row r="41" x14ac:dyDescent="0.2"/>
-    <row r="42" x14ac:dyDescent="0.2"/>
-    <row r="43" x14ac:dyDescent="0.2"/>
-    <row r="44" x14ac:dyDescent="0.2"/>
-    <row r="45" x14ac:dyDescent="0.2"/>
-    <row r="46" x14ac:dyDescent="0.2"/>
-    <row r="47" x14ac:dyDescent="0.2"/>
-    <row r="48" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
-    <row r="62" x14ac:dyDescent="0.2"/>
-    <row r="63" x14ac:dyDescent="0.2"/>
-    <row r="64" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2"/>
     <row r="65" x14ac:dyDescent="0.2"/>
     <row r="66" x14ac:dyDescent="0.2"/>
     <row r="67" x14ac:dyDescent="0.2"/>
@@ -3197,6 +3451,9 @@
       <c r="A1000" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A17" r:id="rId1" xr:uid="{3B2BC5A4-8EF6-4290-B88F-2E7EF401AAF3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>